<commit_message>
Jalon 3 start - taches placed
</commit_message>
<xml_diff>
--- a/outputs/results/results_instance_WPY_simple.xlsx
+++ b/outputs/results/results_instance_WPY_simple.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Taches machine" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Voies utilisation" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Taches humaines" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1113,7 +1115,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1293,7 +1295,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1413,7 +1415,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1653,7 +1655,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>22:15</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1713,7 +1715,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>22:15</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1923,7 +1925,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -2043,7 +2045,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -2080,6 +2082,4173 @@
         <v>15</v>
       </c>
       <c r="F55" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Taux max voies (%)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre max voies occupées</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre total voies dispo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>WPY_REC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>13.33333333333333</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>WPY_FOR</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>WPY_DEP</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>14.28571428571429</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F127"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Id tâche</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Type de tâche</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jour</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Heure début</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Durée</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Sillon</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DEB_A1_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DEB_A1_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10:15</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DEB_A1_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DEB_A3_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DEB_A3_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>22:15</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DEB_A3_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>DEB_A2_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DEB_A2_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>DEB_A2_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>13:15</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>DEB_A2_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>DEB_A2_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>DEB_A2_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>DEB_A3_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>DEB_A3_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>22:15</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>DEB_A3_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>DEB_A1_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>DEB_A1_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>10:15</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>DEB_A1_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>DEB_A3_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>DEB_A3_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>22:15</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>DEB_A3_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>DEB_A1_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>DEB_A1_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>10:15</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>DEB_A1_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>12:45</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>DEB_A2_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>DEB_A2_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>DEB_A2_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>DEB_A2_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>DEB_A2_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>DEB_A2_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>DEB_A1_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>DEB_A1_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>10:15</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>DEB_A1_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>DEB_A3_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>DEB_A3_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>22:15</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>DEB_A3_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>DEB_A2_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>DEB_A2_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>DEB_A2_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>DEB_A3_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>DEB_A3_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>22:15</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>DEB_A3_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>DEB_A1_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>DEB_A1_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>10:15</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>DEB_A1_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>DEB_A3_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>DEB_A3_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>22:15</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>DEB_A3_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>DEB_A4_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>08:45</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>DEB_A4_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>DEB_A4_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>09:45</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>DEB_A4_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>08:45</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>DEB_A4_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>['2' '45' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>DEB_A4_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_REC']</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>09:45</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>FOR_D1_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>FOR_D1_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>FOR_D1_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>FOR_D1_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>FOR_D2_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>FOR_D2_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>14:15</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>FOR_D2_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>FOR_D2_08/08/2022</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>08/08/2022</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>FOR_D1_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>FOR_D1_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>FOR_D1_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>FOR_D1_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>FOR_D3_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>FOR_D3_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>00:15</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>FOR_D3_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>FOR_D3_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>03:30</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>FOR_D2_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>FOR_D2_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>14:15</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>FOR_D2_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>16:45</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>FOR_D2_09/08/2022</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>09/08/2022</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>FOR_D1_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>FOR_D1_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>FOR_D1_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>FOR_D1_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>FOR_D2_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>FOR_D2_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>FOR_D2_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>FOR_D2_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>FOR_D3_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>FOR_D3_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>00:30</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>FOR_D3_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>FOR_D3_10/08/2022</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>10/08/2022</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>03:30</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>FOR_D3_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>FOR_D3_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>00:15</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>FOR_D3_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>FOR_D3_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>03:30</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>FOR_D1_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>FOR_D1_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>14:45</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>FOR_D1_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>FOR_D1_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>FOR_D2_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>FOR_D2_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>14:15</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>FOR_D2_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>22:15</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>FOR_D2_11/08/2022</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>11/08/2022</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>FOR_D2_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>19:15</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>FOR_D2_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>FOR_D2_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>FOR_D2_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>FOR_D1_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>14:15</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>FOR_D1_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>FOR_D1_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>FOR_D1_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>FOR_D3_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>FOR_D3_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>00:30</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>FOR_D3_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>FOR_D3_12/08/2022</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>12/08/2022</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>03:30</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>FOR_D3_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>FOR_D3_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>00:15</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>FOR_D3_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>FOR_D3_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>03:30</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>FOR_D4_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>FOR_D4_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>10:15</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>FOR_D4_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>21:45</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>FOR_D4_13/08/2022</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>13/08/2022</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>FOR_D3_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>FOR_D3_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>00:15</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>FOR_D3_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>FOR_D3_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>03:30</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>FOR_D4_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>['1' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>FOR_D4_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>['2' '150' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>10:15</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>FOR_D4_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>['3' '15' 'WPY_FOR']</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>21:45</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>FOR_D4_14/08/2022</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>['4' '20' 'WPY_DEP']</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>14/08/2022</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
         <is>
           <t>D4</t>
         </is>

</xml_diff>